<commit_message>
Make LinqToSql db context. Move RelationshipDTOs into DTOs and rename to Relationship. After that, change namespace of inside files.
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C88E4C-B7FA-44DC-A181-24C95E384E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C3DEB3-AE10-4C5A-8C60-45CC26E80A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="K15" sqref="K15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LinqToEntityLayer add usecase: UserRole
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C3DEB3-AE10-4C5A-8C60-45CC26E80A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DAAE36-EE38-416A-875E-C631FA676003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="2" r:id="rId1"/>
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:L15"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LinqToEntityLayer add usecase: Promotion
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DAAE36-EE38-416A-875E-C631FA676003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F845197-5ECB-44A4-B1FD-FE153A830564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="871" firstSheet="3" activeTab="17" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="227">
   <si>
     <t>users</t>
   </si>
@@ -739,6 +739,9 @@
   </si>
   <si>
     <t>Mã phân biệt logs</t>
+  </si>
+  <si>
+    <t>Cho phép avatar, thumnail, hashedpassword, salt nullable</t>
   </si>
 </sst>
 </file>
@@ -1352,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F9BB4E-7F92-4A6D-A007-36249FFAD80B}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3464,8 +3467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C0ADA5-CD21-4173-9041-3BD25A88A2EC}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3764,6 +3767,9 @@
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>226</v>
+      </c>
       <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LinqToEntityLayer add usecase: Event
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F845197-5ECB-44A4-B1FD-FE153A830564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC004B5-F9F6-4D1A-A4F6-403F581E9DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="871" firstSheet="3" activeTab="17" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="2" r:id="rId1"/>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F9BB4E-7F92-4A6D-A007-36249FFAD80B}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3467,7 +3467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C0ADA5-CD21-4173-9041-3BD25A88A2EC}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LinqToEntityLayer modify some filters and all services
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC004B5-F9F6-4D1A-A4F6-403F581E9DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AD6E22-9504-4645-AE61-1C9541235B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" firstSheet="3" activeTab="17" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="2" r:id="rId1"/>
@@ -1034,10 +1034,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1355,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F9BB4E-7F92-4A6D-A007-36249FFAD80B}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:Q31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1719,7 @@
       <c r="P21" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="Q21" s="51" t="s">
+      <c r="Q21" s="54" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1752,7 +1752,7 @@
       <c r="P22" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="Q22" s="45" t="s">
+      <c r="Q22" s="28" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1770,7 +1770,7 @@
       <c r="L23" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="Q23" s="52" t="s">
+      <c r="Q23" s="51" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2073,20 +2073,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="E2" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="54" t="s">
+      <c r="E2" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="53" t="s">
         <v>225</v>
       </c>
     </row>
@@ -3467,8 +3467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C0ADA5-CD21-4173-9041-3BD25A88A2EC}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DatabaseEntity Set Avatar, HashedPassword, Salt, Thumnail nullable = true; Set Bill - Total, afterVat, RealPay nullable = false; Set Bill - Total, afterVat, RealPay default values; Re-Migration update database.
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AD6E22-9504-4645-AE61-1C9541235B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B0A0B-0DD8-4005-94C8-D2BE50978DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" firstSheet="3" activeTab="17" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="229">
   <si>
     <t>users</t>
   </si>
@@ -741,7 +741,13 @@
     <t>Mã phân biệt logs</t>
   </si>
   <si>
-    <t>Cho phép avatar, thumnail, hashedpassword, salt nullable</t>
+    <t>Set Bill - Total, afterVat, RealPay nullable = false</t>
+  </si>
+  <si>
+    <t>Set Avatar, HashedPassword, Salt, Thumnail nullable = true</t>
+  </si>
+  <si>
+    <t>Set Bill - Total, afterVat, RealPay default values</t>
   </si>
 </sst>
 </file>
@@ -3468,7 +3474,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3768,16 +3774,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
+      <c r="C24" s="3" t="s">
+        <v>226</v>
+      </c>
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
+      <c r="C25" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>

</xml_diff>

<commit_message>
Modify 202110022237388_ZiCoffeeDb.cs; Update database. Edit documents.
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B0A0B-0DD8-4005-94C8-D2BE50978DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECE08BE-F474-472D-AE67-73B5EE3A6D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" firstSheet="3" activeTab="17" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="225">
   <si>
     <t>users</t>
   </si>
@@ -729,9 +729,6 @@
     <t>datetime2</t>
   </si>
   <si>
-    <t>defaultValue for parentId and descripotion in migration</t>
-  </si>
-  <si>
     <t>LogId</t>
   </si>
   <si>
@@ -739,22 +736,13 @@
   </si>
   <si>
     <t>Mã phân biệt logs</t>
-  </si>
-  <si>
-    <t>Set Bill - Total, afterVat, RealPay nullable = false</t>
-  </si>
-  <si>
-    <t>Set Avatar, HashedPassword, Salt, Thumnail nullable = true</t>
-  </si>
-  <si>
-    <t>Set Bill - Total, afterVat, RealPay default values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,6 +827,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1007,9 +1002,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1044,6 +1036,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1380,235 +1375,235 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="38" t="s">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="20" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="45" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="27" t="s">
+      <c r="Q3" s="26" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="40" t="s">
+      <c r="L4" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="27" t="s">
+      <c r="Q4" s="26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="12"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="41" t="s">
+      <c r="L5" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="29" t="s">
+      <c r="Q5" s="28" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>101</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="12"/>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="26" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="12"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="12"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="12"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="12"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="12"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="12"/>
     </row>
     <row r="17" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="12"/>
@@ -1621,215 +1616,215 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K19" s="31" t="s">
+      <c r="K19" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="21" t="s">
+      <c r="L19" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="M19" s="38" t="s">
+      <c r="M19" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="N19" s="21" t="s">
+      <c r="N19" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="P19" s="21" t="s">
+      <c r="P19" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="Q19" s="21" t="s">
+      <c r="Q19" s="20" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="25" t="s">
         <v>62</v>
       </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="45" t="s">
+      <c r="I20" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="K20" s="32" t="s">
+      <c r="K20" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="L20" s="45" t="s">
+      <c r="L20" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="M20" s="39" t="s">
+      <c r="M20" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="N20" s="45" t="s">
+      <c r="N20" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="P20" s="26" t="s">
+      <c r="P20" s="25" t="s">
         <v>73</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="46" t="s">
+      <c r="G21" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="45" t="s">
+      <c r="I21" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="47" t="s">
+      <c r="K21" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="L21" s="45" t="s">
+      <c r="L21" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="M21" s="49" t="s">
+      <c r="M21" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="N21" s="45" t="s">
+      <c r="N21" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="P21" s="24" t="s">
+      <c r="P21" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="Q21" s="54" t="s">
+      <c r="Q21" s="53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="K22" s="48" t="s">
+      <c r="K22" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="L22" s="36" t="s">
+      <c r="L22" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="M22" s="50" t="s">
+      <c r="M22" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="N22" s="30" t="s">
+      <c r="N22" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="P22" s="30" t="s">
+      <c r="P22" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="Q22" s="28" t="s">
+      <c r="Q22" s="27" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="30" t="s">
+      <c r="I23" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="Q23" s="51" t="s">
+      <c r="Q23" s="50" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="26" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="26" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H26" s="26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="27" t="s">
+      <c r="H27" s="26" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="H28" s="28" t="s">
+      <c r="H28" s="27" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="29" t="s">
+      <c r="H29" s="28" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="29" t="s">
+      <c r="E30" s="28" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2079,21 +2074,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" s="52" t="s">
         <v>224</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>220</v>
-      </c>
-      <c r="E2" s="53" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="53" t="s">
-        <v>202</v>
-      </c>
-      <c r="H2" s="53" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3125,7 +3120,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3474,7 +3469,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3577,13 +3572,13 @@
       <c r="B4" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="b">
+      <c r="C4" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
@@ -3600,13 +3595,13 @@
       <c r="B5" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="b">
         <v>0</v>
       </c>
       <c r="G5" t="s">
@@ -3623,13 +3618,13 @@
       <c r="B6" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="b">
+      <c r="C6" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="8" t="b">
         <v>0</v>
       </c>
       <c r="F6" t="s">
@@ -3649,13 +3644,13 @@
       <c r="B7" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="b">
+      <c r="C7" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8" t="b">
         <v>0</v>
       </c>
       <c r="G7" t="s">
@@ -3765,31 +3760,24 @@
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
-        <v>222</v>
-      </c>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="8"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
-        <v>227</v>
-      </c>
+      <c r="C23" s="8"/>
       <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="C24" s="3" t="s">
-        <v>226</v>
-      </c>
+      <c r="C24" s="8"/>
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="C25" s="3" t="s">
-        <v>228</v>
-      </c>
+      <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
@@ -3811,6 +3799,7 @@
       <c r="A31" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4020,8 +4009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2B094D-5F3E-4895-8DD7-3D897FD51819}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4294,7 +4283,7 @@
         <v>100</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
         <v>105</v>
@@ -4337,7 +4326,7 @@
         <v>123</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>106</v>
@@ -4403,7 +4392,7 @@
         <v>20</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>107</v>
@@ -4845,7 +4834,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5031,7 +5020,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5250,7 +5239,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5397,7 +5386,7 @@
         <v>123</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>132</v>
@@ -5960,7 +5949,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:H13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modify documents, Add attributes (Content, AccessLevel), modify DTOs, DAOs, Engine Filters of Role and Log
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F3407A-E2C4-42E0-9B1F-42405EA657C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10B4E3D-331A-432A-8D34-345FF7385202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" firstSheet="7" activeTab="20" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" activeTab="10" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="229">
   <si>
     <t>users</t>
   </si>
@@ -733,6 +733,27 @@
   </si>
   <si>
     <t>Mã phân biệt logs</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Loại vai trò</t>
+  </si>
+  <si>
+    <t>AccessLevel</t>
+  </si>
+  <si>
+    <t>0 - S
+1 - Administrator
+2 - Manager
+3 - Stocker
+4 - Bartender
+5 - Cashier
+6 - Basic</t>
+  </si>
+  <si>
+    <t>Nội dung log</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1375,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1517,9 @@
       <c r="A5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="12" t="s">
+        <v>226</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="G5" s="32" t="s">
@@ -1778,6 +1801,9 @@
       </c>
       <c r="H24" s="26" t="s">
         <v>45</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -2014,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11A7D9F-6BD9-462E-9672-25810E0E6BAD}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2143,6 +2169,26 @@
       </c>
       <c r="H5" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4674,7 +4720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C481E95F-5280-4CB7-A9FE-90D7EEB4C7C2}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
@@ -4831,14 +4877,14 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.19921875" customWidth="1"/>
     <col min="2" max="2" width="15.09765625" customWidth="1"/>
-    <col min="3" max="3" width="13.296875" customWidth="1"/>
+    <col min="3" max="3" width="20.3984375" customWidth="1"/>
     <col min="4" max="4" width="12.59765625" customWidth="1"/>
     <col min="5" max="5" width="8.19921875" customWidth="1"/>
     <col min="6" max="6" width="21.19921875" customWidth="1"/>
@@ -4947,8 +4993,28 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+    <row r="5" spans="1:13" ht="96.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modify documents, add PromotionValue for BillDetail, re-migration.
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099FCA50-16D5-481C-B215-D7E415CD8989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED6B852-99D6-47F1-B59F-A61983E48DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" activeTab="10" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" firstSheet="4" activeTab="18" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="229">
   <si>
     <t>users</t>
   </si>
@@ -1375,7 +1375,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1801,6 +1801,9 @@
       </c>
       <c r="H24" s="26" t="s">
         <v>45</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>55</v>
       </c>
       <c r="Q24" t="s">
         <v>225</v>
@@ -2040,7 +2043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11A7D9F-6BD9-462E-9672-25810E0E6BAD}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -3851,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01274056-EC25-44E0-ADB6-817B55D3D272}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3992,7 +3995,27 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -5302,7 +5325,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modify documents fix syntax error (PromotionVulue => PromotionValue). FormOrder update IncreaseOrder and LoadBillDetail. FormCashier update MergeTable and LoadBillDetail.
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED6B852-99D6-47F1-B59F-A61983E48DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D99609-063C-4BCE-85CB-9AB41FE5DB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" firstSheet="4" activeTab="18" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="2" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <t>IsAutoApply</t>
   </si>
   <si>
-    <t>PromotionVulue</t>
-  </si>
-  <si>
     <t>IsPercent</t>
   </si>
   <si>
@@ -754,6 +751,9 @@
   </si>
   <si>
     <t>Nội dung log</t>
+  </si>
+  <si>
+    <t>PromotionValue</t>
   </si>
 </sst>
 </file>
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F9BB4E-7F92-4A6D-A007-36249FFAD80B}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1442,10 +1442,10 @@
         <v>50</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P2" s="31" t="s">
         <v>42</v>
@@ -1518,7 +1518,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1532,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="L5" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q5" s="28" t="s">
         <v>42</v>
@@ -1540,14 +1540,14 @@
     </row>
     <row r="6" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" s="12"/>
       <c r="G6" s="33" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K6" s="29" t="s">
         <v>4</v>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B8" s="12"/>
       <c r="H8" s="26" t="s">
-        <v>55</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -1637,14 +1637,14 @@
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="D19" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H19" s="20" t="s">
         <v>29</v>
@@ -1662,10 +1662,10 @@
         <v>33</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P19" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q19" s="20" t="s">
         <v>34</v>
@@ -1674,10 +1674,10 @@
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="D20" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="44" t="s">
@@ -1690,22 +1690,22 @@
         <v>49</v>
       </c>
       <c r="K20" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L20" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M20" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N20" s="44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -1717,7 +1717,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H21" s="26" t="s">
         <v>13</v>
@@ -1729,13 +1729,13 @@
         <v>13</v>
       </c>
       <c r="L21" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M21" s="48" t="s">
         <v>50</v>
       </c>
       <c r="N21" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P21" s="23" t="s">
         <v>7</v>
@@ -1750,31 +1750,31 @@
         <v>8</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H22" s="26" t="s">
         <v>43</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K22" s="47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L22" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M22" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N22" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P22" s="29" t="s">
         <v>8</v>
       </c>
       <c r="Q22" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -1789,7 +1789,7 @@
         <v>51</v>
       </c>
       <c r="L23" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q23" s="50" t="s">
         <v>17</v>
@@ -1797,16 +1797,16 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E24" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H24" s="26" t="s">
         <v>45</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>55</v>
+        <v>228</v>
       </c>
       <c r="Q24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E28" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H28" s="27" t="s">
         <v>10</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="29" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H29" s="28" t="s">
         <v>48</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="30" spans="1:17" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E30" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -1887,60 +1887,60 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1948,7 +1948,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -1957,10 +1957,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1968,19 +1968,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2064,57 +2064,57 @@
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" s="52" t="s">
         <v>222</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>220</v>
-      </c>
-      <c r="E2" s="52" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="52" t="s">
-        <v>202</v>
-      </c>
-      <c r="H2" s="52" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2122,33 +2122,33 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2156,42 +2156,42 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" t="s">
         <v>153</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2276,57 +2276,57 @@
         <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2334,39 +2334,39 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2451,85 +2451,85 @@
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2538,21 +2538,21 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -2561,10 +2561,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2652,57 +2652,57 @@
         <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2710,36 +2710,36 @@
         <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2827,88 +2827,88 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2917,10 +2917,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3007,60 +3007,60 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -3077,10 +3077,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3088,19 +3088,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3186,57 +3186,57 @@
         <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3244,7 +3244,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -3253,21 +3253,21 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3276,10 +3276,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
@@ -3287,10 +3287,10 @@
         <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3299,21 +3299,21 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3322,10 +3322,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3333,10 +3333,10 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -3345,10 +3345,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3356,22 +3356,22 @@
         <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3379,33 +3379,33 @@
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3414,47 +3414,47 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
     </row>
     <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H15" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3535,40 +3535,40 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3576,16 +3576,16 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3593,22 +3593,22 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3616,10 +3616,10 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" s="8">
         <v>0</v>
@@ -3628,10 +3628,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3639,10 +3639,10 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
@@ -3651,10 +3651,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3662,10 +3662,10 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" s="8">
         <v>0</v>
@@ -3674,13 +3674,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3688,10 +3688,10 @@
         <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7" s="8">
         <v>0</v>
@@ -3700,10 +3700,10 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
@@ -3711,10 +3711,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3723,10 +3723,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3734,22 +3734,22 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3757,16 +3757,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3774,16 +3774,16 @@
         <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3854,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01274056-EC25-44E0-ADB6-817B55D3D272}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3875,40 +3875,40 @@
         <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3916,16 +3916,16 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3933,27 +3933,27 @@
         <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3962,10 +3962,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3973,10 +3973,10 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3985,24 +3985,24 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -4011,10 +4011,10 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4096,40 +4096,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4137,16 +4137,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4154,7 +4154,7 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -4163,10 +4163,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4174,7 +4174,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -4183,10 +4183,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -4194,7 +4194,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -4203,18 +4203,18 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -4223,13 +4223,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -4237,7 +4237,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7">
         <v>50</v>
@@ -4246,13 +4246,13 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -4260,7 +4260,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -4269,10 +4269,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -4280,7 +4280,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -4289,10 +4289,10 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -4300,19 +4300,19 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -4320,22 +4320,22 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -4343,7 +4343,7 @@
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -4352,10 +4352,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
@@ -4363,10 +4363,10 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4375,10 +4375,10 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -4386,22 +4386,22 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -4409,7 +4409,7 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -4418,13 +4418,13 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -4432,7 +4432,7 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -4441,10 +4441,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4452,7 +4452,7 @@
         <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -4461,18 +4461,18 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -4485,7 +4485,7 @@
         <v>18</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
@@ -4493,7 +4493,7 @@
         <v>19</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
@@ -4501,15 +4501,15 @@
         <v>20</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4522,7 +4522,7 @@
         <v>3</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -4530,7 +4530,7 @@
         <v>4</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -4538,7 +4538,7 @@
         <v>5</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -4551,7 +4551,7 @@
         <v>36</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4609,43 +4609,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4653,33 +4653,33 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4764,40 +4764,40 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4805,16 +4805,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4822,16 +4822,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4920,40 +4920,40 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4961,7 +4961,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -4970,10 +4970,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" t="s">
         <v>202</v>
-      </c>
-      <c r="H2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4981,7 +4981,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -4990,10 +4990,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -5001,30 +5001,30 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="110.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -5033,10 +5033,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -5125,40 +5125,40 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5166,16 +5166,16 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5183,7 +5183,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -5192,10 +5192,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -5203,19 +5203,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
@@ -5223,10 +5223,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5235,10 +5235,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -5246,7 +5246,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -5255,10 +5255,10 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -5325,7 +5325,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5345,40 +5345,40 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5386,16 +5386,16 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5403,7 +5403,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -5412,10 +5412,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -5423,19 +5423,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
@@ -5443,10 +5443,10 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5455,33 +5455,33 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -5489,10 +5489,10 @@
         <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -5501,21 +5501,21 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -5524,10 +5524,10 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -5535,16 +5535,16 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -5626,57 +5626,57 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5684,7 +5684,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -5693,10 +5693,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -5704,7 +5704,7 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -5713,10 +5713,10 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -5724,7 +5724,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="14">
         <v>11</v>
@@ -5733,10 +5733,10 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -5744,7 +5744,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -5753,15 +5753,15 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H9" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -5786,7 +5786,7 @@
         <v>3</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -5794,7 +5794,7 @@
         <v>4</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -5863,57 +5863,57 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5921,7 +5921,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -5930,10 +5930,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -5941,7 +5941,7 @@
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -5950,21 +5950,21 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -5973,10 +5973,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -6055,40 +6055,40 @@
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6096,16 +6096,16 @@
         <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6113,7 +6113,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -6122,10 +6122,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -6133,7 +6133,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -6142,16 +6142,16 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C5" s="14"/>
       <c r="H5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -6231,40 +6231,40 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6272,16 +6272,16 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6289,7 +6289,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -6298,10 +6298,10 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="41.4" x14ac:dyDescent="0.25">
@@ -6309,10 +6309,10 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -6321,10 +6321,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -6332,17 +6332,17 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" s="14"/>
       <c r="E5" t="b">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add attributes (Code, AppliedTime) for DiscountDetail (Entity, configuration, migration, provider, filter, model, service). FormCheckout fix lsvDiscountDetail. Add enum PromotionTypes. Make imageList for lsvDiscountDetail.
</commit_message>
<xml_diff>
--- a/Documents/DatabaseTemplate.xlsx
+++ b/Documents/DatabaseTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZiCoffee\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D99609-063C-4BCE-85CB-9AB41FE5DB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35040725-C294-46C4-A97C-76913CC371A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" tabRatio="871" xr2:uid="{73728B45-DF20-4BB7-9DD1-83E67F2630F4}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="234">
   <si>
     <t>users</t>
   </si>
@@ -754,6 +754,21 @@
   </si>
   <si>
     <t>PromotionValue</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>AppliedDate</t>
+  </si>
+  <si>
+    <t>Mã voucher/coupon được áp dụng (nếu có)</t>
+  </si>
+  <si>
+    <t>Thời gian áp dụng chương trình khuyến mãi</t>
+  </si>
+  <si>
+    <t>AppliedTime</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1390,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1752,6 +1767,9 @@
       <c r="E22" s="26" t="s">
         <v>200</v>
       </c>
+      <c r="G22" t="s">
+        <v>229</v>
+      </c>
       <c r="H22" s="26" t="s">
         <v>43</v>
       </c>
@@ -1781,6 +1799,9 @@
       <c r="A23" s="11"/>
       <c r="E23" s="26" t="s">
         <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>233</v>
       </c>
       <c r="H23" s="26" t="s">
         <v>44</v>
@@ -4592,7 +4613,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4683,7 +4704,44 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>